<commit_message>
Feature/my order sync (#6)
* Added Al orders

* WIP: Added my order changes
</commit_message>
<xml_diff>
--- a/backend/data/settlements.xlsx
+++ b/backend/data/settlements.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T5"/>
+  <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -670,9 +670,62 @@
         <v>2025-07-22T00:49:46.757Z</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>settlement_1753294282531_mmatj9jez</v>
+      </c>
+      <c r="B6" t="str">
+        <v>user_1753125931723_8ftkkx2pf</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Adarsh</v>
+      </c>
+      <c r="D6">
+        <v>9.97</v>
+      </c>
+      <c r="E6" t="str">
+        <v>lucky@okaxis</v>
+      </c>
+      <c r="F6" t="str">
+        <v>ORD-001,ORD-002,ORD-004</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6" t="str">
+        <v>INR</v>
+      </c>
+      <c r="I6" t="str">
+        <v>approved</v>
+      </c>
+      <c r="J6" t="str">
+        <v>settled_partially</v>
+      </c>
+      <c r="K6" t="str">
+        <v>2025-07-23T18:11:22.531Z</v>
+      </c>
+      <c r="L6" t="str">
+        <v>2025-07-23T18:11:57.047Z</v>
+      </c>
+      <c r="M6">
+        <v>5</v>
+      </c>
+      <c r="N6" t="str">
+        <v>111</v>
+      </c>
+      <c r="O6" t="str">
+        <v>payment-proof-1753294317020-14169049.webp</v>
+      </c>
+      <c r="P6" t="str">
+        <v>user_1753040616422_hgtapju6r</v>
+      </c>
+      <c r="Q6" t="str">
+        <v>2025-07-23T18:11:57.043Z</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:T5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:T6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>